<commit_message>
se agrega segundo paso
</commit_message>
<xml_diff>
--- a/bondad_ajuste_frisby.xlsx
+++ b/bondad_ajuste_frisby.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,166 +436,301 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Tipo</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>Distribución</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>K-S (p)</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>A-D (stat)</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Tipo</t>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Evaluación Visual</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Decisión Final</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Letra Notación</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>Tiempos entre llegadas</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
           <t>Exponencial</t>
         </is>
       </c>
-      <c r="B2" t="n">
+      <c r="C2" t="n">
         <v>0.2077624555612785</v>
       </c>
-      <c r="C2" t="n">
+      <c r="D2" t="n">
         <v>1.704538857752482</v>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Llegadas</t>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Aceptable</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>✅ Se acepta</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>M</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>Tiempos entre llegadas</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
           <t>Normal</t>
         </is>
       </c>
-      <c r="B3" t="n">
+      <c r="C3" t="n">
         <v>9.908539415492668e-05</v>
       </c>
-      <c r="C3" t="n">
-        <v>7.983629470097142</v>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Llegadas</t>
+      <c r="D3" t="n">
+        <v>7.983629470097156</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Malo</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>❌ Se descarta</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>N</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>Tiempos entre llegadas</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
           <t>Lognormal</t>
         </is>
       </c>
-      <c r="B4" t="n">
+      <c r="C4" t="n">
         <v>0.3599305001028352</v>
       </c>
-      <c r="C4" t="n">
+      <c r="D4" t="n">
         <v>0.9790362244201276</v>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Llegadas</t>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Aceptable</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>✅ Se acepta</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>G</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>Tiempos entre llegadas</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
           <t>Gamma</t>
         </is>
       </c>
-      <c r="B5" t="n">
+      <c r="C5" t="n">
         <v>5.955649589091438e-112</v>
       </c>
-      <c r="C5" t="n">
+      <c r="D5" t="n">
         <v>1.704538857752482</v>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Llegadas</t>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Malo</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>❌ Se descarta</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>G</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>Tiempos de servicio</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
           <t>Exponencial</t>
         </is>
       </c>
-      <c r="B6" t="n">
+      <c r="C6" t="n">
         <v>0.001432964130728354</v>
       </c>
-      <c r="C6" t="n">
+      <c r="D6" t="n">
         <v>18.68980018452545</v>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Servicio</t>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Malo</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>❌ Se descarta</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>M</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>Tiempos de servicio</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
           <t>Normal</t>
         </is>
       </c>
-      <c r="B7" t="n">
+      <c r="C7" t="n">
         <v>0.0638398959041292</v>
       </c>
-      <c r="C7" t="n">
-        <v>4.148560891450501</v>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Servicio</t>
+      <c r="D7" t="n">
+        <v>4.148560891450487</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>✅ Se acepta</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>N</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>Tiempos de servicio</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
           <t>Lognormal</t>
         </is>
       </c>
-      <c r="B8" t="n">
+      <c r="C8" t="n">
         <v>0.950008058207393</v>
       </c>
-      <c r="C8" t="n">
+      <c r="D8" t="n">
         <v>0.4870928663281546</v>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Servicio</t>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Excelente</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>✅ Se acepta</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>G</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>Tiempos de servicio</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
           <t>Gamma</t>
         </is>
       </c>
-      <c r="B9" t="n">
+      <c r="C9" t="n">
         <v>0.6267300574370787</v>
       </c>
-      <c r="C9" t="n">
+      <c r="D9" t="n">
         <v>18.68980018452545</v>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>Servicio</t>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Bueno</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>✅ Se acepta</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>G</t>
         </is>
       </c>
     </row>

</xml_diff>